<commit_message>
added the new view of the data.
</commit_message>
<xml_diff>
--- a/public/Content_Scout.xlsx
+++ b/public/Content_Scout.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B27F8EE-BE24-47BD-80B6-09770A96742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{0B27F8EE-BE24-47BD-80B6-09770A96742A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25039F9C-F165-44D9-8973-13AEEC6E5CA1}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="39">
   <si>
     <t>Hashtags</t>
   </si>
@@ -94,10 +94,23 @@
     <t>Note</t>
   </si>
   <si>
+    <t>apify filter</t>
+  </si>
+  <si>
     <t>String</t>
   </si>
   <si>
-    <t>words must be comma seperated else will be considered as one</t>
+    <t>words must be comma seperated else will be considered as one , TikTok hashtags   scraper will collect data about videos containing this hashtag: likes, users, followers and more.
+You can enter the hashtags one by one with comma seperated.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>Organic / ads</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
   <si>
     <t>proper language words must be insterted ,Only 1 language be provided at a time.  eg-&gt; German/ English</t>
@@ -106,16 +119,16 @@
     <t>number</t>
   </si>
   <si>
-    <t>days cout in number , if 0 then will not be considered ,eg-&gt; 5</t>
+    <t>days cout in number , if 0 then will not be considered ,eg-&gt; 5 ,  Only videos uploaded after the days of how old the scraped videos should be in days. Putting 1 will get you only today's posts, 2 - yesterday's and today's, and so on.</t>
   </si>
   <si>
     <t>views cout in number , if 0 then will not be considered ,eg-&gt; 5</t>
   </si>
   <si>
-    <t>Like cout in number , if 0 then will not be considered ,eg-&gt; 5</t>
-  </si>
-  <si>
-    <t>Count cout in number , if 0 then will not be considered ,eg-&gt; 5</t>
+    <t>Like cout in number , if 0 then will not be considered ,eg-&gt; 5, Scrapes only profiles with min like on the profile.</t>
+  </si>
+  <si>
+    <t>Count cout in number , if 0 then will not be considered ,eg-&gt; 5, Scrapes only profiles with min comment on the profile.</t>
   </si>
   <si>
     <r>
@@ -148,13 +161,22 @@
     </r>
   </si>
   <si>
+    <t>Min. follower in number , if 0 then will not be considered ,eg-&gt; 5, Scrapes only profiles with more then  number on followers in the profile</t>
+  </si>
+  <si>
+    <t>Depend on filte of likes , if passeed then have to extract at out system</t>
+  </si>
+  <si>
+    <t>Max. follower in number , if 0 then will not be considered ,eg-&gt; 5,  Scrapes only profiles with more then  number on followers in the profile</t>
+  </si>
+  <si>
     <t>Min. follower in number , if 0 then will not be considered ,eg-&gt; 5</t>
   </si>
   <si>
-    <t>Max. follower in number , if 0 then will not be considered ,eg-&gt; 5</t>
-  </si>
-  <si>
     <t xml:space="preserve">country string if need result from specific country , else will be on empty no country filter will be applied. </t>
+  </si>
+  <si>
+    <t>words must be comma seperated else will be considered as one, Your keyword will apply to both videos description and user profiles.</t>
   </si>
 </sst>
 </file>
@@ -664,16 +686,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2F1C32-5366-4FCD-BC4D-D295E29FC233}">
   <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="26.7109375" customWidth="1"/>
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
@@ -692,16 +713,22 @@
       <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" ht="29.25">
+      <c r="D1" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="101.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
       </c>
       <c r="G2" s="1"/>
       <c r="L2" s="2"/>
@@ -711,7 +738,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="43.5">
@@ -719,21 +752,27 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="29.25">
+        <v>26</v>
+      </c>
+      <c r="D4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="87">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="29.25">
@@ -741,32 +780,41 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
         <v>23</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="29.25">
+    </row>
+    <row r="7" spans="1:12" ht="43.5">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="29.25">
+    </row>
+    <row r="8" spans="1:12" ht="43.5">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" t="s">
         <v>23</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="72.75">
@@ -774,32 +822,41 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
         <v>23</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="29.25">
+    </row>
+    <row r="10" spans="1:12" ht="57.75">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="29.25">
+        <v>33</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="57.75">
       <c r="A11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>30</v>
+        <v>35</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="29.25">
@@ -807,10 +864,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D12" t="s">
         <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="43.5">
@@ -818,21 +878,27 @@
         <v>11</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="29.25">
+        <v>37</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="57.75">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>